<commit_message>
update for the python builtin annotation such as property, staticmethod, classmethod
</commit_message>
<xml_diff>
--- a/01_hello_world/files/xls_temp.xlsx
+++ b/01_hello_world/files/xls_temp.xlsx
@@ -1516,14 +1516,65 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1597,52 +1648,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>